<commit_message>
Added updated provider metadata to Mac Low, new file names for an object
</commit_message>
<xml_diff>
--- a/mac-low/provider_metadata/AV_Container_List.xlsx
+++ b/mac-low/provider_metadata/AV_Container_List.xlsx
@@ -3943,9 +3943,6 @@
     <t>MSS0180_B243_F07</t>
   </si>
   <si>
-    <t>MSS0180_B243_F08_1, MSS0180_B243_F08_2</t>
-  </si>
-  <si>
     <t>MSS0180_B243_F09</t>
   </si>
   <si>
@@ -4067,6 +4064,9 @@
   </si>
   <si>
     <t>MSS0180_B244_F12_1, MSS0180_B244_F12_2</t>
+  </si>
+  <si>
+    <t>MSS0180_B243_F08_1, MSS0180_B243_F08_2, MSS0180_B243_F08_3, MSS0180_B243_F08_4</t>
   </si>
 </sst>
 </file>
@@ -6302,8 +6302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="81" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="G265" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="81" workbookViewId="0">
+      <selection activeCell="V272" sqref="V272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9700,7 +9700,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>641</v>
       </c>
@@ -9747,7 +9747,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>641</v>
       </c>
@@ -19870,7 +19870,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="271" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
         <v>641</v>
       </c>
@@ -19914,7 +19914,7 @@
         <v>187</v>
       </c>
       <c r="U271" s="5" t="s">
-        <v>1297</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="272" spans="1:22" x14ac:dyDescent="0.25">
@@ -19958,7 +19958,7 @@
         <v>643</v>
       </c>
       <c r="U272" s="5" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="273" spans="1:22" x14ac:dyDescent="0.25">
@@ -20005,7 +20005,7 @@
         <v>188</v>
       </c>
       <c r="U273" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="274" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -20052,7 +20052,7 @@
         <v>941</v>
       </c>
       <c r="U274" s="5" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="275" spans="1:22" x14ac:dyDescent="0.25">
@@ -20099,7 +20099,7 @@
         <v>941</v>
       </c>
       <c r="U275" s="5" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="276" spans="1:22" x14ac:dyDescent="0.25">
@@ -20146,7 +20146,7 @@
         <v>942</v>
       </c>
       <c r="U276" s="5" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="277" spans="1:22" x14ac:dyDescent="0.25">
@@ -20193,7 +20193,7 @@
         <v>950</v>
       </c>
       <c r="U277" s="5" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="278" spans="1:22" x14ac:dyDescent="0.25">
@@ -20240,7 +20240,7 @@
         <v>943</v>
       </c>
       <c r="U278" s="5" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="279" spans="1:22" x14ac:dyDescent="0.25">
@@ -20287,7 +20287,7 @@
         <v>944</v>
       </c>
       <c r="U279" s="5" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="280" spans="1:22" x14ac:dyDescent="0.25">
@@ -20331,7 +20331,7 @@
         <v>643</v>
       </c>
       <c r="U280" s="5" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="281" spans="1:22" x14ac:dyDescent="0.25">
@@ -20378,7 +20378,7 @@
         <v>6</v>
       </c>
       <c r="U281" s="5" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="V281" s="5" t="s">
         <v>1005</v>
@@ -20434,7 +20434,7 @@
         <v>941</v>
       </c>
       <c r="U282" s="5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="V282" s="5" t="s">
         <v>1005</v>
@@ -20487,7 +20487,7 @@
         <v>8</v>
       </c>
       <c r="U283" s="5" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="284" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -20540,7 +20540,7 @@
         <v>941</v>
       </c>
       <c r="U284" s="5" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="285" spans="1:22" x14ac:dyDescent="0.25">
@@ -20593,7 +20593,7 @@
         <v>941</v>
       </c>
       <c r="U285" s="5" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="286" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -20646,7 +20646,7 @@
         <v>941</v>
       </c>
       <c r="U286" s="5" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="287" spans="1:22" x14ac:dyDescent="0.25">
@@ -20696,7 +20696,7 @@
         <v>941</v>
       </c>
       <c r="U287" s="5" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="288" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -20749,7 +20749,7 @@
         <v>941</v>
       </c>
       <c r="U288" s="5" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="289" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -20802,7 +20802,7 @@
         <v>941</v>
       </c>
       <c r="U289" s="5" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="290" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -20855,7 +20855,7 @@
         <v>941</v>
       </c>
       <c r="U290" s="5" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="291" spans="1:21" x14ac:dyDescent="0.25">
@@ -20908,7 +20908,7 @@
         <v>941</v>
       </c>
       <c r="U291" s="5" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="292" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -20958,7 +20958,7 @@
         <v>17</v>
       </c>
       <c r="U292" s="5" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="293" spans="1:21" x14ac:dyDescent="0.25">
@@ -21008,7 +21008,7 @@
         <v>18</v>
       </c>
       <c r="U293" s="5" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="294" spans="1:21" x14ac:dyDescent="0.25">
@@ -21061,7 +21061,7 @@
         <v>941</v>
       </c>
       <c r="U294" s="5" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="295" spans="1:21" x14ac:dyDescent="0.25">
@@ -21111,7 +21111,7 @@
         <v>20</v>
       </c>
       <c r="U295" s="5" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="296" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -21161,7 +21161,7 @@
         <v>21</v>
       </c>
       <c r="U296" s="5" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="297" spans="1:21" x14ac:dyDescent="0.25">
@@ -21208,7 +21208,7 @@
         <v>22</v>
       </c>
       <c r="U297" s="5" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="298" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -21261,7 +21261,7 @@
         <v>941</v>
       </c>
       <c r="U298" s="5" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="299" spans="1:21" x14ac:dyDescent="0.25">
@@ -21311,7 +21311,7 @@
         <v>941</v>
       </c>
       <c r="U299" s="5" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="300" spans="1:21" x14ac:dyDescent="0.25">
@@ -21355,7 +21355,7 @@
         <v>955</v>
       </c>
       <c r="U300" s="5" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="301" spans="1:21" x14ac:dyDescent="0.25">
@@ -21402,7 +21402,7 @@
         <v>956</v>
       </c>
       <c r="U301" s="5" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="302" spans="1:21" x14ac:dyDescent="0.25">
@@ -21447,7 +21447,7 @@
         <v>957</v>
       </c>
       <c r="U302" s="5" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="303" spans="1:21" x14ac:dyDescent="0.25">
@@ -21494,7 +21494,7 @@
         <v>959</v>
       </c>
       <c r="U303" s="5" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="304" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -21538,7 +21538,7 @@
         <v>643</v>
       </c>
       <c r="U304" s="5" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="305" spans="1:22" x14ac:dyDescent="0.25">
@@ -21585,7 +21585,7 @@
         <v>962</v>
       </c>
       <c r="U305" s="5" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="306" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -21629,7 +21629,7 @@
       <c r="R306" s="11"/>
       <c r="S306" s="11"/>
       <c r="U306" s="11" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="V306" s="11"/>
     </row>
@@ -21677,7 +21677,7 @@
         <v>964</v>
       </c>
       <c r="U307" s="5" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="308" spans="1:22" x14ac:dyDescent="0.25">
@@ -21724,7 +21724,7 @@
         <v>966</v>
       </c>
       <c r="U308" s="5" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="309" spans="1:22" x14ac:dyDescent="0.25">
@@ -21771,7 +21771,7 @@
         <v>970</v>
       </c>
       <c r="U309" s="5" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="310" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -21818,7 +21818,7 @@
       <c r="S310" s="11"/>
       <c r="T310" s="5"/>
       <c r="U310" s="11" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="V310" s="11"/>
     </row>
@@ -21866,7 +21866,7 @@
         <v>974</v>
       </c>
       <c r="U311" s="5" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="312" spans="1:22" x14ac:dyDescent="0.25">
@@ -21906,7 +21906,7 @@
         <v>643</v>
       </c>
       <c r="U312" s="5" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="V312" s="5" t="s">
         <v>941</v>

</xml_diff>